<commit_message>
ex_05 korrigiert und ex_06 begonnen
</commit_message>
<xml_diff>
--- a/ex_05/jacobi/scripts/Jacobi.xlsx
+++ b/ex_05/jacobi/scripts/Jacobi.xlsx
@@ -56,8 +56,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -2077,7 +2076,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2093,7 +2092,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
@@ -2102,675 +2101,611 @@
       <c r="N1"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>256</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" si="0">A2*A2*8</f>
         <v>524288</v>
       </c>
-      <c r="C2" s="3">
-        <v>1157.190793</v>
-      </c>
-      <c r="D2" s="3">
-        <v>697.16206</v>
+      <c r="C2">
+        <v>1129.6001779999999</v>
+      </c>
+      <c r="D2">
+        <v>1003.5137590000001</v>
       </c>
       <c r="I2"/>
-      <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
-      <c r="M2"/>
       <c r="N2"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>299</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
         <v>715208</v>
       </c>
-      <c r="C3" s="3">
-        <v>1097.3572879999999</v>
-      </c>
-      <c r="D3" s="3">
-        <v>736.83719099999996</v>
+      <c r="C3">
+        <v>1118.4014560000001</v>
+      </c>
+      <c r="D3">
+        <v>1030.0562179999999</v>
       </c>
       <c r="I3"/>
-      <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="M3"/>
       <c r="N3"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>350</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
         <v>980000</v>
       </c>
-      <c r="C4" s="3">
-        <v>1136.682483</v>
-      </c>
-      <c r="D4" s="3">
-        <v>774.67281700000001</v>
+      <c r="C4">
+        <v>1151.4905639999999</v>
+      </c>
+      <c r="D4">
+        <v>1047.896508</v>
       </c>
       <c r="I4"/>
-      <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
-      <c r="M4"/>
       <c r="N4"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>409</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>1338248</v>
       </c>
-      <c r="C5" s="3">
-        <v>1110.3628189999999</v>
-      </c>
-      <c r="D5" s="3">
-        <v>802.81501100000003</v>
+      <c r="C5">
+        <v>1122.2351209999999</v>
+      </c>
+      <c r="D5">
+        <v>1004.83805</v>
       </c>
       <c r="I5"/>
-      <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="M5"/>
       <c r="N5"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>478</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>1827872</v>
       </c>
-      <c r="C6" s="3">
-        <v>1110.2999259999999</v>
-      </c>
-      <c r="D6" s="3">
-        <v>834.50105199999996</v>
+      <c r="C6">
+        <v>1103.901245</v>
+      </c>
+      <c r="D6">
+        <v>1005.58543</v>
       </c>
       <c r="I6"/>
-      <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
-      <c r="M6"/>
       <c r="N6"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>559</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>2499848</v>
       </c>
-      <c r="C7" s="3">
-        <v>1138.7539139999999</v>
-      </c>
-      <c r="D7" s="3">
-        <v>892.93587500000001</v>
+      <c r="C7">
+        <v>1138.864133</v>
+      </c>
+      <c r="D7">
+        <v>1033.974007</v>
       </c>
       <c r="I7"/>
-      <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
-      <c r="M7"/>
       <c r="N7"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>654</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>3421728</v>
       </c>
-      <c r="C8" s="3">
-        <v>1184.5816090000001</v>
-      </c>
-      <c r="D8" s="3">
-        <v>933.361985</v>
+      <c r="C8">
+        <v>1171.2437339999999</v>
+      </c>
+      <c r="D8">
+        <v>1065.205213</v>
       </c>
       <c r="I8"/>
-      <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
-      <c r="M8"/>
       <c r="N8"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>765</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>4681800</v>
       </c>
-      <c r="C9" s="3">
-        <v>1144.33889</v>
-      </c>
-      <c r="D9" s="3">
-        <v>943.18356100000005</v>
+      <c r="C9">
+        <v>1145.1203310000001</v>
+      </c>
+      <c r="D9">
+        <v>1038.6963189999999</v>
       </c>
       <c r="I9"/>
-      <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
-      <c r="M9"/>
       <c r="N9"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>895</v>
       </c>
       <c r="B10">
         <f t="shared" ref="B10:B33" si="1">A10*A10*8</f>
         <v>6408200</v>
       </c>
-      <c r="C10" s="3">
-        <v>1103.1109060000001</v>
-      </c>
-      <c r="D10" s="3">
-        <v>953.872435</v>
+      <c r="C10">
+        <v>1096.6893689999999</v>
+      </c>
+      <c r="D10">
+        <v>1026.5049610000001</v>
       </c>
       <c r="I10"/>
-      <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
-      <c r="M10"/>
       <c r="N10"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>1047</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
         <v>8769672</v>
       </c>
-      <c r="C11" s="3">
-        <v>955.88675000000001</v>
-      </c>
-      <c r="D11" s="3">
-        <v>856.92601000000002</v>
+      <c r="C11">
+        <v>960.74203999999997</v>
+      </c>
+      <c r="D11">
+        <v>894.91907400000002</v>
       </c>
       <c r="I11"/>
-      <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
-      <c r="M11"/>
       <c r="N11"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>1224</v>
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
         <v>11985408</v>
       </c>
-      <c r="C12" s="3">
-        <v>912.75928799999997</v>
-      </c>
-      <c r="D12" s="3">
-        <v>855.13901499999997</v>
+      <c r="C12">
+        <v>910.14231099999995</v>
+      </c>
+      <c r="D12">
+        <v>873.31736599999999</v>
       </c>
       <c r="I12"/>
-      <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
-      <c r="M12"/>
       <c r="N12"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>1432</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
         <v>16404992</v>
       </c>
-      <c r="C13" s="3">
-        <v>639.37661600000001</v>
-      </c>
-      <c r="D13" s="3">
-        <v>465.19892700000003</v>
+      <c r="C13">
+        <v>650.57595500000002</v>
+      </c>
+      <c r="D13">
+        <v>641.89950299999998</v>
       </c>
       <c r="I13"/>
-      <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
-      <c r="M13"/>
       <c r="N13"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>1674</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
         <v>22418208</v>
       </c>
-      <c r="C14" s="3">
-        <v>587.44833200000005</v>
-      </c>
-      <c r="D14" s="3">
-        <v>577.43222800000001</v>
+      <c r="C14">
+        <v>583.48600199999998</v>
+      </c>
+      <c r="D14">
+        <v>572.89033700000005</v>
       </c>
       <c r="I14"/>
-      <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
-      <c r="M14"/>
       <c r="N14"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>1958</v>
       </c>
       <c r="B15">
         <f t="shared" si="1"/>
         <v>30670112</v>
       </c>
-      <c r="C15" s="3">
-        <v>560.88391799999999</v>
-      </c>
-      <c r="D15" s="3">
-        <v>561.57662600000003</v>
+      <c r="C15">
+        <v>558.30220999999995</v>
+      </c>
+      <c r="D15">
+        <v>557.99654399999997</v>
       </c>
       <c r="I15"/>
-      <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
-      <c r="M15"/>
       <c r="N15"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>2290</v>
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
         <v>41952800</v>
       </c>
-      <c r="C16" s="3">
-        <v>585.79559200000006</v>
-      </c>
-      <c r="D16" s="3">
-        <v>577.554891</v>
+      <c r="C16">
+        <v>584.49718399999995</v>
+      </c>
+      <c r="D16">
+        <v>577.63206300000002</v>
       </c>
       <c r="I16"/>
-      <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
-      <c r="M16"/>
       <c r="N16"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>2678</v>
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
         <v>57373472</v>
       </c>
-      <c r="C17" s="3">
-        <v>582.34519299999999</v>
-      </c>
-      <c r="D17" s="3">
-        <v>572.37581999999998</v>
+      <c r="C17">
+        <v>573.69523700000002</v>
+      </c>
+      <c r="D17">
+        <v>570.80249900000001</v>
       </c>
       <c r="I17"/>
-      <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
-      <c r="M17"/>
       <c r="N17"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>3132</v>
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
         <v>78475392</v>
       </c>
-      <c r="C18" s="3">
-        <v>565.87723800000003</v>
-      </c>
-      <c r="D18" s="3">
-        <v>552.54212800000005</v>
+      <c r="C18">
+        <v>564.05833099999995</v>
+      </c>
+      <c r="D18">
+        <v>560.28959799999996</v>
       </c>
       <c r="I18"/>
-      <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
-      <c r="M18"/>
       <c r="N18"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>3662</v>
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
         <v>107281952</v>
       </c>
-      <c r="C19" s="3">
-        <v>587.39065900000003</v>
-      </c>
-      <c r="D19" s="3">
-        <v>579.10484899999994</v>
+      <c r="C19">
+        <v>586.66232400000001</v>
+      </c>
+      <c r="D19">
+        <v>582.57688800000005</v>
       </c>
       <c r="I19"/>
-      <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="M19"/>
       <c r="N19"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>4283</v>
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
         <v>146752712</v>
       </c>
-      <c r="C20" s="3">
-        <v>581.22129800000005</v>
-      </c>
-      <c r="D20" s="3">
-        <v>580.78039699999999</v>
+      <c r="C20">
+        <v>584.93781899999999</v>
+      </c>
+      <c r="D20">
+        <v>581.19653000000005</v>
       </c>
       <c r="I20"/>
-      <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-      <c r="M20"/>
       <c r="N20"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>5009</v>
       </c>
       <c r="B21">
         <f t="shared" si="1"/>
         <v>200720648</v>
       </c>
-      <c r="C21" s="3">
-        <v>579.33366899999999</v>
-      </c>
-      <c r="D21" s="3">
-        <v>578.11170600000003</v>
+      <c r="C21">
+        <v>575.59313699999996</v>
+      </c>
+      <c r="D21">
+        <v>572.65296799999999</v>
       </c>
       <c r="I21"/>
-      <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
-      <c r="M21"/>
       <c r="N21"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>5857</v>
       </c>
       <c r="B22">
         <f t="shared" si="1"/>
         <v>274435592</v>
       </c>
-      <c r="C22" s="3">
-        <v>576.02370900000005</v>
-      </c>
-      <c r="D22" s="3">
-        <v>574.20469200000002</v>
+      <c r="C22">
+        <v>570.65314999999998</v>
+      </c>
+      <c r="D22">
+        <v>573.30922299999997</v>
       </c>
       <c r="I22"/>
-      <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="M22"/>
       <c r="N22"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>6850</v>
       </c>
       <c r="B23">
         <f t="shared" si="1"/>
         <v>375380000</v>
       </c>
-      <c r="C23" s="3">
-        <v>583.79478500000005</v>
-      </c>
-      <c r="D23" s="3">
-        <v>584.11791900000003</v>
+      <c r="C23">
+        <v>582.296964</v>
+      </c>
+      <c r="D23">
+        <v>563.417913</v>
       </c>
       <c r="I23"/>
-      <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
-      <c r="M23"/>
       <c r="N23"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>8011</v>
       </c>
       <c r="B24">
         <f t="shared" si="1"/>
         <v>513408968</v>
       </c>
-      <c r="C24" s="3">
-        <v>528.79411300000004</v>
-      </c>
-      <c r="D24" s="3">
-        <v>529.46957699999996</v>
+      <c r="C24">
+        <v>527.47463900000002</v>
+      </c>
+      <c r="D24">
+        <v>537.488516</v>
       </c>
       <c r="I24"/>
-      <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
-      <c r="M24"/>
       <c r="N24"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>9368</v>
       </c>
       <c r="B25">
         <f t="shared" si="1"/>
         <v>702075392</v>
       </c>
-      <c r="C25" s="3">
-        <v>489.35463199999998</v>
-      </c>
-      <c r="D25" s="3">
-        <v>484.83450800000003</v>
+      <c r="C25">
+        <v>486.61191700000001</v>
+      </c>
+      <c r="D25">
+        <v>551.43946400000004</v>
       </c>
       <c r="I25"/>
-      <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
-      <c r="M25"/>
       <c r="N25"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>10955</v>
       </c>
       <c r="B26">
         <f t="shared" si="1"/>
         <v>960096200</v>
       </c>
-      <c r="C26" s="3">
-        <v>491.93533600000001</v>
-      </c>
-      <c r="D26" s="3">
-        <v>490.17258700000002</v>
+      <c r="C26">
+        <v>487.590169</v>
+      </c>
+      <c r="D26">
+        <v>567.97750699999995</v>
       </c>
       <c r="I26"/>
-      <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
-      <c r="M26"/>
       <c r="N26"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>12811</v>
       </c>
       <c r="B27">
         <f t="shared" si="1"/>
         <v>1312973768</v>
       </c>
-      <c r="C27" s="3">
-        <v>474.70011199999999</v>
-      </c>
-      <c r="D27" s="3">
-        <v>546.90570500000001</v>
+      <c r="C27">
+        <v>473.68696699999998</v>
+      </c>
+      <c r="D27">
+        <v>521.60547599999995</v>
       </c>
       <c r="I27"/>
-      <c r="J27"/>
       <c r="K27"/>
       <c r="L27"/>
-      <c r="M27"/>
       <c r="N27"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>14982</v>
       </c>
       <c r="B28">
         <f t="shared" si="1"/>
         <v>1795682592</v>
       </c>
-      <c r="C28" s="3">
-        <v>481.03057000000001</v>
-      </c>
-      <c r="D28" s="3">
-        <v>654.43081500000005</v>
+      <c r="C28">
+        <v>481.99663099999998</v>
+      </c>
+      <c r="D28">
+        <v>563.41983200000004</v>
       </c>
       <c r="I28"/>
-      <c r="J28"/>
       <c r="K28"/>
       <c r="L28"/>
-      <c r="M28"/>
       <c r="N28"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>17521</v>
       </c>
       <c r="B29">
         <f t="shared" si="1"/>
         <v>2455883528</v>
       </c>
-      <c r="C29" s="3">
-        <v>483.934099</v>
-      </c>
-      <c r="D29" s="3">
-        <v>768.37998200000004</v>
+      <c r="C29">
+        <v>483.21789200000001</v>
+      </c>
+      <c r="D29">
+        <v>566.92242699999997</v>
       </c>
       <c r="I29"/>
-      <c r="J29"/>
       <c r="K29"/>
       <c r="L29"/>
-      <c r="M29"/>
       <c r="N29"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>20489</v>
       </c>
       <c r="B30">
         <f t="shared" si="1"/>
         <v>3358392968</v>
       </c>
-      <c r="C30" s="3">
-        <v>488.79403000000002</v>
-      </c>
-      <c r="D30" s="3">
-        <v>909.421606</v>
+      <c r="C30">
+        <v>486.71804500000002</v>
+      </c>
+      <c r="D30">
+        <v>537.69910700000003</v>
       </c>
       <c r="I30"/>
-      <c r="J30"/>
       <c r="K30"/>
       <c r="L30"/>
-      <c r="M30"/>
       <c r="N30"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>23961</v>
       </c>
       <c r="B31">
         <f t="shared" si="1"/>
         <v>4593036168</v>
       </c>
-      <c r="C31" s="3">
-        <v>477.909378</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1055.668887</v>
+      <c r="C31">
+        <v>472.272626</v>
+      </c>
+      <c r="D31">
+        <v>544.11497499999996</v>
       </c>
       <c r="I31"/>
-      <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
-      <c r="M31"/>
       <c r="N31"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>28021</v>
       </c>
       <c r="B32">
         <f t="shared" si="1"/>
         <v>6281411528</v>
       </c>
-      <c r="C32" s="3">
-        <v>480.27801299999999</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1229.8799690000001</v>
+      <c r="C32">
+        <v>476.49312900000001</v>
+      </c>
+      <c r="D32">
+        <v>549.31219899999996</v>
       </c>
       <c r="I32"/>
-      <c r="J32"/>
       <c r="K32"/>
       <c r="L32"/>
-      <c r="M32"/>
       <c r="N32"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>32768</v>
       </c>
       <c r="B33">
         <f t="shared" si="1"/>
         <v>8589934592</v>
       </c>
-      <c r="C33" s="3">
-        <v>474.15587399999998</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1415.523342</v>
+      <c r="C33">
+        <v>467.83911000000001</v>
+      </c>
+      <c r="D33">
+        <v>517.53895499999999</v>
       </c>
       <c r="I33"/>
-      <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
-      <c r="M33"/>
       <c r="N33"/>
     </row>
     <row r="35" ht="14.25"/>

</xml_diff>